<commit_message>
Agregar informacion a hoja de consolidado
</commit_message>
<xml_diff>
--- a/Proyecto Pago Seguridad Social/django_project_pss/media/plantillas/Consolidado.xlsx
+++ b/Proyecto Pago Seguridad Social/django_project_pss/media/plantillas/Consolidado.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>EMPLEADO</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>TOTAL EMPLEADO</t>
+  </si>
+  <si>
+    <t>TOTAL PATRON</t>
   </si>
 </sst>
 </file>
@@ -490,7 +493,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.140625" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -563,7 +566,7 @@
         <v>14</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Agregar formato de moneda a los totales
</commit_message>
<xml_diff>
--- a/Proyecto Pago Seguridad Social/django_project_pss/media/plantillas/Consolidado.xlsx
+++ b/Proyecto Pago Seguridad Social/django_project_pss/media/plantillas/Consolidado.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>EMPLEADO</t>
   </si>
   <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
     <t>PATRON</t>
   </si>
   <si>
@@ -65,6 +62,12 @@
   </si>
   <si>
     <t>TOTAL PATRON</t>
+  </si>
+  <si>
+    <t>PLANILLA</t>
+  </si>
+  <si>
+    <t>TOTAL P.</t>
   </si>
 </sst>
 </file>
@@ -490,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.140625" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -508,7 +511,7 @@
     <col min="15" max="16384" width="19.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="6" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D1" s="7" t="s">
         <v>0</v>
       </c>
@@ -516,7 +519,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
@@ -525,51 +528,54 @@
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
     </row>
-    <row r="2" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se añade rubro temporal y permanente a consolidado
</commit_message>
<xml_diff>
--- a/Proyecto Pago Seguridad Social/django_project_pss/media/plantillas/Consolidado.xlsx
+++ b/Proyecto Pago Seguridad Social/django_project_pss/media/plantillas/Consolidado.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20340"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE0154D-9B8F-4323-8CBF-03D3BAA7D34D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237F6490-390D-4F12-8798-02FEF701B928}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>EMPLEADO</t>
   </si>
@@ -26,9 +26,6 @@
     <t>NIT</t>
   </si>
   <si>
-    <t xml:space="preserve">RUBRO </t>
-  </si>
-  <si>
     <t>CONCEPTO</t>
   </si>
   <si>
@@ -78,6 +75,12 @@
   </si>
   <si>
     <t>UNIDAD 9</t>
+  </si>
+  <si>
+    <t>RUBRO TEMPORAL</t>
+  </si>
+  <si>
+    <t>RUBRO PERMANENTE</t>
   </si>
 </sst>
 </file>
@@ -583,107 +586,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.140625" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="19.140625" style="1"/>
-    <col min="8" max="8" width="22.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21" style="1" customWidth="1"/>
-    <col min="10" max="10" width="23" style="1" customWidth="1"/>
-    <col min="11" max="11" width="26.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="27.85546875" style="1" customWidth="1"/>
-    <col min="13" max="14" width="27.5703125" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="19.140625" style="1"/>
+    <col min="1" max="8" width="19.140625" style="1"/>
+    <col min="9" max="9" width="22.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23" style="1" customWidth="1"/>
+    <col min="12" max="12" width="26.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="27.85546875" style="1" customWidth="1"/>
+    <col min="14" max="15" width="27.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="19.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="6" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="6" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="9"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="7"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="7"/>
+      <c r="I1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
-      <c r="O1" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="O1" s="7"/>
       <c r="P1" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="J2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>13</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="H1:N1"/>
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>